<commit_message>
alerta hecha para coordenadas no recibidas
</commit_message>
<xml_diff>
--- a/Coordenadas.xlsx
+++ b/Coordenadas.xlsx
@@ -1,88 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\OneDrive\Documentos\UNI\TERCERO\CRIPTO\proyecto_cripto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C318C9B-AF7A-4CA2-AC6C-87DB2107D0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Nickname</t>
-  </si>
-  <si>
-    <t>Key_symmetric</t>
-  </si>
-  <si>
-    <t>Coordenadas</t>
-  </si>
-  <si>
-    <t>Luffy</t>
-  </si>
-  <si>
-    <t>b'F\x16v2\xbb\xe1"\x8c\x04s\xb2*\x957K\xe1z\x02&gt;M\x7f\x07\xda\xa8I\x86:\' :\xa8\x0f\xcb\x97\xaf\x8f4\xd6?&amp;\x0f\xef\xf8%\x96{EGE\xe7F\x97e\x91\xdbPmC\xc1w~\x96\xb0A\xcef\xb7\x12%\r4NLS\x06&gt;\x1c\xbc\xb8U\x824\x8a\xe8\xafPau]\'^?h\xa6\x17K\xcb!\xe4\x04CfS\xe7\x02\x16\xd1EsF\r&gt;\x86\tP\xaa-\xa5\x89\r\xb8\xb2G\xe0h\xa62\xe6r|\x8b\xf5\xbd\x93bzK\xc1\xec\x19\xe9\x16/\xbd)Ef\xc9\xad\x84\x8a\xbf\xaeyf\r\x16\xd7\xffK\xb3h\xd9+*\xaf\xb3\xbeB\xd0\x10*\xd7\xd5\x19.r\xbe.z\xf4lSq9\xb5A\xdej\xce=U\xad\xf7_mz3\xe6\xe5R)\x10\x0e\xee\xe2\tP\xa5`\xcd\x068\x08\x98\x89\xb4(\x82e\x83\x1b\xf4\x06\xb8/\x9f?\xf9\xe53VzK_\xae{t@P\xce4\xc9\xcb\nR\xf6\xe8\xd79\xa5j\xde\r\x9cI'</t>
-  </si>
-  <si>
-    <t>b'gAAAAABlNulwl57UPR2nFW4ep293W7eF2DM1VWmeJiQCvkXBOnocaVTNnzCI1E39QUgKxfy8IOBbciCat4rEsFEaRGpsLIr_-Q=='</t>
-  </si>
-  <si>
-    <t>Nami</t>
-  </si>
-  <si>
-    <t>Maripili</t>
-  </si>
-  <si>
-    <t>Sanji</t>
-  </si>
-  <si>
-    <t>Usopp</t>
-  </si>
-  <si>
-    <t>Zoro</t>
-  </si>
-  <si>
-    <t>Shanks</t>
-  </si>
-  <si>
-    <t>Arlong</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -97,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,71 +420,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="118.44140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nickname</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Key_symmetric</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Coordenadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Luffy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>b"6\t\xb1\xce\x87\xbf\xb7\x1e\x8b\x072\x0f\xd1\x1f\x0e\xf1\x00\x9d\xb7\x18SV\x08\xcah8kVU\xeer\xc2{rz\xde\xf4\xca\xfb\x91j]\xa0x\x19e.1\xe4\xbf\x94\xa5[af\x94V&amp;~\x9bc\x80\x85{\xc4Q\x11-\xf9\xc9F[R\n\xa6\xe1IF\xbc&amp;}5\x04\xfa\x9f)\xf3g\xe4A\xad\x971R%\xe2UH\xec\r\x97\x85\xb0\t\x8b\xb4\xda\xa6[\xf7R%\x99E&amp;Z\xe7h^\xe2\xe2\xf4#&gt;&gt;\xe9\xf81\x91\xce\xee6\x98\x02\x06.-b\xa5\x0c\x7f\x1e\tP\x97\x05&amp;\xdc\xcbKA\x88R\xa6\xce\xee\x10_s\xce5'~\x884q\r\x9e\x1a\xf3jj\x05\xa1m\xb4\xae\xf1\x06$\xe0&amp;\xd6&gt;\xc4\x12z\xa4\xa4U?\xf4\xea\x04m\xf3\xb5\x15\xa1\xe06\xa8?!I\xd9\xb4\x88\x0b\xbdL\xd8E9\xd1\xc1!\xe02V\xcf\n\xef\x00\xb1/\x89\xd0iu\xcd\x0f\x8f5@\xa9YE\x8fX\x05\xe5\x8f\xec6\x0fW1\x95\xd5\xf8 \xc1\x9d\xd5="</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>b'gAAAAABlN6NwZ_VQOx-hfNyv_dmEVDL61N8koRV9RrP9c6X8MuHG0eHci4i6yimtkh1rmZeKYe2KL7Pz7C_ozFpplxWZxDLN9A=='</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Nami</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>b"\x8f,\x1c}\xee\xf7U\x97'?\xdeIN13\xd5)U\xf3\xa1\xac\xe7\xa1\x9e\xd2vY\xbc\xdb\xc0\x8bPluM\x13\x93\xbe\x7f\xcd\xbaK\x1b\\/\x1dq\xd0\xa2\xb1Y8\x91|\xb8\xcd\xf6\x04\xa1\xb1\xf1\x13\x9dP\x12\x03\x1d$\x83\x10\x82\xabDh\n\xb6{\xcc\xad\xf9\xe8\xba\xbb\xd5\x8e4F\x8f\xb1zu\xa0\x19\x11/\xd4\x0e\xa2qE\x10o\x9ce\x18:\x88\xedG\xbe?\x058\x0ew\xf1\xb9S}\x0b\xa6\x83pC\xb0\xc0\x94\x90/\xa4\xb3\\\x0c\x0c\xd6\r!\xf1\xd9\x9b#0\xe5C\xf2\x92\x85\xaf\xaae\xe2\x0e\xe0\xe5\xfbT\x9b_o\x0f6\xe0\xc3\xf3\xf4\xe5\xd4\x88\xad\x18\xda\xcf\xe3\x8dtSF|i\xdc\x9aYi\xb3\xb0\x03DH\xd0\x9c\xf7\xcb\xc5\x0f@\x85\x1a\xa6\xde\xd4\x07f\xdd~\r\x0ba^\xa6\x95|\xc4\xf4_!\x11\xad\xd9\x8ag\xa3\xbfx\x8d\xff8|\xa1e(\x0b\xb7\x18Fzg:\xb6X|\x80kt\x8d\xf0\xc7r-q\xf0\xcfC\x18\xc7\xa0\xaf"</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>b'gAAAAABlOYb-YOXjn9VXrFRbH6wZ4LosZBkORriGiAV4B1HxI2FThXPXOGmmbea_MtD4gxmkotJfVcJ3b1sOlwQ7nuBRdR_KmQ=='</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Maripili</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sanji</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Usopp</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Zoro</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Shanks</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Arlong</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>b'#\xeb\xc2U\xd5\xbb\x7f\xfb\x0f,39\xa4)#\r)\x0e\x01\x87t\x0b\xb9@\'\xc5\xcd\x90]=\xee\xf0\xe4\x1ca\\\x15\n$2\xccb\x1b9\xe0J\xa7L \x95\xf4PGL\xf1\x17+\xa0u\x0f5eQa\x9dp\x92\xe5\xf8\x8e,xO\xd2\xd0/"L\xd4\x1c\xf0a/\t\x91\xf9\xc0\x91\x81\xff.@D\xa8\xf0\xec\xf81\x03\xbf\x13\x10\xd3\x99\x8f\xfc\xb5\xba\xe2\x19\xb6\xa7^+\xb0&lt;=\xd3+E\xd8R4" [J\xb6z\x15L}0\x12\xec\xed\xf2\xc5\xde\x14\xea\x98p7\xd3\xd8-\x9a\x8av0\xa4&gt;\xf2{\x1b\xd6\x19\xdb\x07M\x1fv\xf2A\x11\xdf&lt;g\xa0\xa2:3\xa5\xf6x\xbdb^\x1cJ\x0b\xa8~\xb6\xf5\xff\x16\x11n\xe5g\xe5J4\xc1\xbf\xe5\xc3\xec\'^(*\xd6C\xe3\xf6\xe1;\x8b4\xc98X9OM`\xeb\xbf\x07\x13p\xe0\xaa\x9c\x92\xa6\x16"x\\\xa8\xb4\nw0\xb9\xde\x0e\xa7\xaa\xaa\xc4\x13WL\xdd\x98k\xe7\xfd\xf3\x92['</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>b'gAAAAABlNvDQYh94aBoH2mvXEItIY2MKasvxU8c6exQD4oDKxRo1qUXa93RQmhYIYkfBMrXVMuSqacyZwJdm2GTuuFGSfxvs0w=='</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Código listo para entregar
</commit_message>
<xml_diff>
--- a/Coordenadas.xlsx
+++ b/Coordenadas.xlsx
@@ -490,8 +490,16 @@
           <t>Maripili</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>b"+\x8d\xffM\xe1Ti\xd1S^\xc4s\xc4\xec\xaegF\x03hB|NWLm\xcb[\xc9\xcb\x9c\x9ei\xa5\xbb|\x9d\x84['\xb91\x83\x90\x1e\xd2K\xf2[\x035\x9e\xeb\xf7\xa3\x93\xf5\xb0&amp;&lt;\xe6v\x96\x89\x8e\xb8?%\x82\\\xca\xe7oV\x0c\xadU\xd2\x9b\x00\x1b#\xe07\x8c\xed\xfc\xb2\xb5{\xcb)\xd49\xaf\x99\xac^\xc3\xdbO\x0bR\xbfZ&amp;\xa5\x8b^\xe5\x7f\x0e\xc5\x04\xac\xa4\x97\x17\xeaC\x1a\xf2\xc0[7\x81Z\x02\xe7\xae\xf7e3[\xf9py\xde\xdf4\xd3\xea\x868R\xe4\tSPqN\xa4\xd6.Z\xe37\xf8\n\xfa\x84\x94R\xfa\x9dX\x06F\xa5SF}h\xab\x93\xc0$\xb7\xe7\x1b(\xe6\x98.\x14/\x7f\xca\x83\xf6\x8c\xd7J\xc9\x0e\xaf\x03B&amp;\xeaB=f\x98\xe2\x92L\x91\xa0n\x89:\xf1g\xeb%\xaeUK(\xba\xc6\xbef\x16zehG\xea=\xaaS\xc4o\xae|\x08\xf5\xbe]T\x8dd\xef\xa4L-N\xe8D\n\x0c\xe5\xb4y\xa8"</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>b'gAAAAABlOtRCmpIkP4Z9uUZnV8kFi6TSCh4UnjqS7_t3qfft3lLKmjOLzrauGuXgD2gnN_sjIa5YzEBsrt2wSQDJBNpBYu03Qg=='</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -499,8 +507,16 @@
           <t>Sanji</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>b'\x15H\xd3\xd3\xcf\xec|\xf6\xac\xf9\xd3\xe9\xe9\x94\xf1\xeaa-T\x9f\xc2.e\x15\xafd\xd1\xce=L\xc9\xc3\xe8\x1e4-\xd3R\x9a\xc6\xa5X-\x16a2w\x0fz\xcbFw\x9f\x1f\xcePf\xbb\xf8\x88\xdeA\xfd\xba\x14J\x9dC\xe3\x7f&gt;\x94F\xcf\x0bh\xa7$\xcd\xaeNI)\xa2\xe4&lt;\xfe&amp;\xce\x8a\x94`N8;\xd3\x18\xe4\x1c`\x82J&gt;\xd2\xae\x8f\xae\xd4\xce\xc7\x96\xcdeb\x15VA\x99\xc93\x0f/\xeb\xf6\x9f\x19|\xb0\xf6\x98\xb1\xc9\xb3\x99u\xb3&lt;\x17*\x92%\xb5\x13s\xe5\xf4\xb0$n\xa9Q\x9b\xeb\x1f\x8f\t_\x0f\xaf{\xa0i\xfd\xda\x8a\xa5$\xc4\x89\x90\x99b\x1a\xdc\xe5\xca{f\x12\xde\x06\xc0orJ\xeaH\xa5H\xfb\xbb\xb8\x8c5zV\xa4N\xc29\xf0\xa8\x9a\xaemC\x853\xda\x15\x01\xa6\xaa5I\xb0+\xa6\xa7\x02&lt;\x9c\x11\x1a\xe0\x7f_\xf0\xa9\x1d0v\xa2s3f\x9ds\x83\xb1l\xba\xf0O\x80D\xa6\xf8\xd0F\xf1\xf3\x04L\x9d '</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>b'gAAAAABlOtPiomb0JFqbBEbxYATf_cEGJXa7OTvG5QaKI1o_XQuA91Yi7lw1xc2cGFEzMGJL4p1rOYLoOmD_zg9aLZK6YIUmybt5dSNE1plcxb2QJBXkBdw='</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">

</xml_diff>